<commit_message>
le journal de bord mis a jour
</commit_message>
<xml_diff>
--- a/paperasse/journal de bord.xlsx
+++ b/paperasse/journal de bord.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="28515" windowHeight="12600"/>
@@ -11,21 +11,12 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
-  <si>
-    <t>commencer rfepartition tache</t>
-  </si>
-  <si>
-    <t>creation BDD sans valeur</t>
-  </si>
-  <si>
-    <t>Gant grossièrement fait</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>date</t>
   </si>
@@ -36,76 +27,16 @@
     <t>difficulté rencontré</t>
   </si>
   <si>
-    <t>difficulté trouver but du mini projet</t>
-  </si>
-  <si>
-    <t>révision de la BDD &amp; ajout de quelque valeurs</t>
-  </si>
-  <si>
-    <t>commencer comprention matos</t>
-  </si>
-  <si>
-    <t>connexion a la BDD faites dans l'index (possiblement a deplacer)</t>
-  </si>
-  <si>
-    <t>que linterface donner ?</t>
-  </si>
-  <si>
-    <t>automatisation de la connexion</t>
-  </si>
-  <si>
-    <t>mis le projet sur GIT</t>
-  </si>
-  <si>
-    <t>gant complété</t>
-  </si>
-  <si>
-    <t>Ajout de liens a la BDD et rerévision</t>
-  </si>
-  <si>
-    <t>commencement a intégrer un formlaire connexion &amp; inscription</t>
-  </si>
-  <si>
-    <t>API rest en reflexion &amp; non fonctionnel</t>
-  </si>
-  <si>
-    <t>que mettre dans l'API rest</t>
-  </si>
-  <si>
-    <t>des liens dans la BDD difficile a comprendre</t>
-  </si>
-  <si>
-    <t>idcompte champ de tableau invalide (liens mal fait)</t>
-  </si>
-  <si>
-    <t>page inscription/connexion fonctionnel</t>
-  </si>
-  <si>
-    <t>page de planning fonctionnel</t>
-  </si>
-  <si>
-    <t>preparation doc pour présentation oral au client</t>
-  </si>
-  <si>
-    <t>la page du scanner fontionne</t>
-  </si>
-  <si>
-    <t>perte du journal de bord a partir de 07/10/2021 mais pas code</t>
-  </si>
-  <si>
-    <t>page reommé pour ne plus être administrateur, gérant et formateur</t>
-  </si>
-  <si>
-    <t>la page de scan est plus difficile a utiliser sans scan</t>
-  </si>
-  <si>
-    <t>l'utilisateur peut cliquer partout sur la page de scan normalement si il scan son réusultat seras affiché si dans la BDD</t>
-  </si>
-  <si>
-    <t>système de sécu couteux en ressource par rapport a la page</t>
-  </si>
-  <si>
     <t>remise en forme du site</t>
+  </si>
+  <si>
+    <t>entrainement QT</t>
+  </si>
+  <si>
+    <t>decouverte QT serial</t>
+  </si>
+  <si>
+    <t>doc de l'arraigné superflue</t>
   </si>
 </sst>
 </file>
@@ -441,7 +372,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -454,7 +385,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1">
         <v>44473</v>
@@ -471,89 +402,31 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
         <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="D9" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B10" s="1">
         <v>44480</v>
@@ -567,35 +440,12 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>